<commit_message>
Updated credentials and fixed authenticator issue
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +491,57 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-01-30 14:02:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>dsds</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-01-30 14:21:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>dfdf</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>from streamlit.hello.dataframe_demo import data_frame_demo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-01-30 14:50:10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Reverted to version without login functionality
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,6 +542,23 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>world</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-01-30 15:18:26</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated app with full-width editable table
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,149 +412,88 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A2:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>World</t>
-        </is>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>2025-01-30 16:03:19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Row</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>hello world</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>140</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Robin</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-01-30 11:27:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TSLA</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-01-30 11:28:51</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-01-30 14:02:13</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>dsds</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-01-30 14:21:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>dfdf</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>from streamlit.hello.dataframe_demo import data_frame_demo</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2025-01-30 14:50:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Hello</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>world</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2025-01-30 15:18:26</t>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Rental Income</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1100</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2034</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2345</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>657</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>657</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>777</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>787</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>788</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>790</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>800</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
commit the updated code to where it needs to be
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -2,16 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Main" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Log" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Main" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -63,7 +62,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -426,120 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:O3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-01-30 16:03:19</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2001</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Rental Income</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1100</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2034</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2345</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>456</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>345</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>657</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>657</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>777</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>787</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>788</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>790</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-02-04 17:12:36</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,243 +505,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Hello worlds</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>100</v>
-      </c>
-      <c r="D2" t="n">
-        <v>123</v>
-      </c>
-      <c r="E2" t="n">
-        <v>200</v>
-      </c>
-      <c r="F2" t="n">
-        <v>3220</v>
-      </c>
-      <c r="G2" t="n">
-        <v>200</v>
-      </c>
-      <c r="H2" t="n">
-        <v>355</v>
-      </c>
-      <c r="I2" t="n">
-        <v>6522</v>
-      </c>
-      <c r="J2" t="n">
-        <v>32</v>
-      </c>
-      <c r="K2" t="n">
-        <v>200</v>
-      </c>
-      <c r="L2" t="n">
-        <v>552</v>
-      </c>
-      <c r="M2" t="n">
-        <v>8555</v>
-      </c>
-      <c r="N2" t="n">
-        <v>6215</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Action</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Updated Data</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-02-04 17:20:07</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{"Account Number":{},"Account Name":{},"January":{},"February":{},"March":{},"April":{},"May":{},"June":{},"July":{},"August":{},"September":{},"October":{},"November":{},"December":{}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-02-04 17:38:39</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{"Account Number":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"Account Name":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"January":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"February":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"March":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"April":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"May":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"June":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"July":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"August":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"September":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"October":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"November":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""},"December":{"0":"","1":"","2":"","3":"","4":"","5":"","6":"","7":""}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-02-04 17:50:51</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>{"Account Number":{"0":"","1":""},"Account Name":{"0":0.0,"1":0.0},"January":{"0":0.0,"1":0.0},"February":{"0":0.0,"1":0.0},"March":{"0":0.0,"1":0.0},"April":{"0":0.0,"1":0.0},"May":{"0":0.0,"1":0.0},"June":{"0":0.0,"1":0.0},"July":{"0":0.0,"1":0.0},"August":{"0":0.0,"1":0.0},"September":{"0":0.0,"1":0.0},"October":{"0":0.0,"1":0.0},"November":{"0":0.0,"1":0.0},"December":{"0":0.0,"1":0.0}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-02-04 17:51:28</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>{"Account Number":{"0":"","1":"","2":""},"Account Name":{"0":null,"1":null,"2":0.0},"January":{"0":null,"1":null,"2":0.0},"February":{"0":null,"1":null,"2":0.0},"March":{"0":null,"1":null,"2":0.0},"April":{"0":null,"1":null,"2":0.0},"May":{"0":null,"1":null,"2":0.0},"June":{"0":null,"1":null,"2":0.0},"July":{"0":null,"1":null,"2":0.0},"August":{"0":null,"1":null,"2":0.0},"September":{"0":null,"1":null,"2":0.0},"October":{"0":null,"1":null,"2":0.0},"November":{"0":null,"1":null,"2":0.0},"December":{"0":null,"1":null,"2":0.0}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-02-04 17:57:36</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>{"Account Number":{"0":"","1":""},"Account Name":{"0":0.0,"1":0.0},"January":{"0":300.0,"1":0.0},"February":{"0":0.0,"1":0.0},"March":{"0":0.0,"1":0.0},"April":{"0":0.0,"1":0.0},"May":{"0":0.0,"1":0.0},"June":{"0":0.0,"1":0.0},"July":{"0":0.0,"1":0.0},"August":{"0":0.0,"1":0.0},"September":{"0":0.0,"1":0.0},"October":{"0":0.0,"1":0.0},"November":{"0":0.0,"1":0.0},"December":{"0":0.0,"1":0.0}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-02-04 18:29:28</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>{"Account Number":{"0":"4854"},"Account Name":{"0":"2343"},"January":{"0":null},"February":{"0":null},"March":{"0":null},"April":{"0":null},"May":{"0":null},"June":{"0":null},"July":{"0":null},"August":{"0":null},"September":{"0":null},"October":{"0":null},"November":{"0":null},"December":{"0":null}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-02-04 18:37:50</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>{"Account Number":{"0":"2834","1":null},"Account Name":{"0":"Hello","1":null},"January":{"0":"20331","1":null},"February":{"0":"20+3","1":null},"March":{"0":"2034","1":null},"April":{"0":"20304","1":null},"May":{"0":"30340","1":null},"June":{"0":"2030","1":null},"July":{"0":"20304","1":null},"August":{"0":"0003","1":null},"September":{"0":"20304","1":null},"October":{"0":"2003","1":null},"November":{"0":"2030","1":null},"December":{"0":"12,26","1":null}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-02-04 18:38:52</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{"Account Number":{"0":"2834","1":"1111","2":null},"Account Name":{"0":"Hello","1":"Hello You","2":null},"January":{"0":"20331","1":"0","2":null},"February":{"0":"20+3","1":"21","2":null},"March":{"0":"2034","1":"2","2":null},"April":{"0":"20304","1":"6","2":null},"May":{"0":"30340","1":"5","2":null},"June":{"0":"2030","1":"8","2":null},"July":{"0":"20304","1":"32","2":null},"August":{"0":"0003","1":"2","2":null},"September":{"0":"20304","1":null,"2":null},"October":{"0":"2003","1":"2","2":null},"November":{"0":"2030","1":"0","2":null},"December":{"0":"12,26","1":"0","2":null}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-02-07 11:51:43</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Update</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>{'Account Number': {0: '1000'}, 'Account Name': {0: 'Hello worlds'}, 'January': {0: 100}, 'February': {0: 123}, 'March': {0: 200}, 'April': {0: 3220}, 'May': {0: 200}, 'June': {0: 355}, 'July': {0: 6522}, 'August': {0: 32}, 'September': {0: 200}, 'October': {0: 552}, 'November': {0: 8555}, 'December': {0: 6215}}</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>